<commit_message>
err now outputs index
</commit_message>
<xml_diff>
--- a/GUI/Reference.xlsx
+++ b/GUI/Reference.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Senior-Design-master\Senior-Design-master\GUI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\Files\Senior_Design\Senior-Design\GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,18 +24,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>qk</t>
   </si>
   <si>
     <t>qh</t>
   </si>
+  <si>
+    <t>xa</t>
+  </si>
+  <si>
+    <t>ya</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -350,7 +356,7 @@
   <dimension ref="A1:D140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -362,6 +368,12 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">

</xml_diff>